<commit_message>
Add GetUnderlyingFactors to simulators Some house keeping.
</commit_message>
<xml_diff>
--- a/ExcelExamples/CreateProductFromFile.xlsx
+++ b/ExcelExamples/CreateProductFromFile.xlsx
@@ -536,17 +536,17 @@
   <dimension ref="B2:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.625" customWidth="1"/>
-    <col min="5" max="5" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.35">
@@ -573,7 +573,7 @@
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="str">
         <f>_xll.QSA.CreateProductFromFile(C3,C4)</f>
-        <v>simpleCallFromFile.20:53:11-21</v>
+        <v>simpleCallFromFile.11:42:19-14</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="21" x14ac:dyDescent="0.35">
@@ -605,7 +605,7 @@
       </c>
       <c r="C14" s="1" t="str">
         <f>Model!B11</f>
-        <v>equitySimulator01.20:53:11-23</v>
+        <v>equitySimulator01.11:42:19-15</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
@@ -619,13 +619,13 @@
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="str">
         <f>_xll.QSA.Value(C12,B8,C13,C14,C15)</f>
-        <v>simpleCallFromFileValue.20:53:12-25</v>
+        <v>simpleCallFromFileValue.11:42:20-18</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="8">
         <f>_xll.QSA.GetResults(B17,"value")</f>
-        <v>1.5830912547608202</v>
+        <v>1.5451465707928331</v>
       </c>
     </row>
   </sheetData>
@@ -643,12 +643,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.625" customWidth="1"/>
-    <col min="5" max="5" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:7" ht="21" x14ac:dyDescent="0.35">
@@ -675,7 +675,7 @@
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="str">
         <f>_xll.QSA.CreateProductFromFile(C4,C5)</f>
-        <v>productFromFile.20:53:13-27</v>
+        <v>productFromFile.11:42:20-17</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="21" x14ac:dyDescent="0.35">
@@ -724,13 +724,13 @@
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="str">
         <f>_xll.QSA.Value(C13,B9,Model!M6,Model!B11,C14)</f>
-        <v>productFromFileValue.20:53:13-28</v>
+        <v>productFromFileValue.11:42:21-20</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="8">
         <f>_xll.QSA.GetResults(B16,"value")</f>
-        <v>1.6391098319403998</v>
+        <v>1.6201430965076</v>
       </c>
     </row>
   </sheetData>
@@ -743,17 +743,17 @@
   <dimension ref="B2:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.625" customWidth="1"/>
-    <col min="5" max="5" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.35">
@@ -780,7 +780,7 @@
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="str">
         <f>_xll.QSA.CreateProductFromFile(C3,C4)</f>
-        <v>incentiveOptionFromFile.20:53:11-24</v>
+        <v>incentiveOptionFromFile.11:42:20-16</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="21" x14ac:dyDescent="0.35">
@@ -812,7 +812,7 @@
       </c>
       <c r="C14" s="1" t="str">
         <f>Model!B11</f>
-        <v>equitySimulator01.20:53:11-23</v>
+        <v>equitySimulator01.11:42:19-15</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
@@ -826,13 +826,13 @@
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="str">
         <f>_xll.QSA.Value(C12,B8,C13,C14,C15)</f>
-        <v>incentiveOptionFromFileValue.20:53:12-26</v>
+        <v>incentiveOptionFromFileValue.11:42:20-19</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="8">
         <f>_xll.QSA.GetResults(B17,"value")</f>
-        <v>38.548253246309351</v>
+        <v>34.538951123841137</v>
       </c>
     </row>
   </sheetData>
@@ -850,14 +850,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="3.875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="21" x14ac:dyDescent="0.35">
@@ -885,7 +885,7 @@
       </c>
       <c r="C4" s="1" t="str">
         <f>M9</f>
-        <v>ZARDiscount.20:53:11-22</v>
+        <v>ZARDiscount.11:42:19-13</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>10</v>
@@ -993,13 +993,13 @@
       </c>
       <c r="M9" s="5" t="str">
         <f>_xll.QSA.CreateDatesAndRatesCurve(N3,M6:M7,N6:N7,N4)</f>
-        <v>ZARDiscount.20:53:11-22</v>
+        <v>ZARDiscount.11:42:19-13</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="str">
         <f>_xll.QSA.CreateEquityModel(C3,C4,B7:B9,C7:C9,D7:D9,E7:E9,G7:I9)</f>
-        <v>equitySimulator01.20:53:11-23</v>
+        <v>equitySimulator01.11:42:19-15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Checks that all example sheets run without error. Fixes any errors that were present. Allows default values in Excel code generation.
</commit_message>
<xml_diff>
--- a/ExcelExamples/CreateProductFromFile.xlsx
+++ b/ExcelExamples/CreateProductFromFile.xlsx
@@ -4,20 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="10290"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="10290" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Script Call Simple" sheetId="5" r:id="rId1"/>
-    <sheet name="Script Call" sheetId="1" r:id="rId2"/>
-    <sheet name="Script Incentive Option" sheetId="3" r:id="rId3"/>
-    <sheet name="Model" sheetId="4" r:id="rId4"/>
+    <sheet name="Script Incentive Option" sheetId="3" r:id="rId2"/>
+    <sheet name="Model" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621" calcMode="manual" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>name</t>
   </si>
@@ -73,18 +72,6 @@
     <t>simulations</t>
   </si>
   <si>
-    <t>QSA.FormulaBlackScholes</t>
-  </si>
-  <si>
-    <t>productFromFile</t>
-  </si>
-  <si>
-    <t>exercise date in script</t>
-  </si>
-  <si>
-    <t>strike in script</t>
-  </si>
-  <si>
     <t>QSA.CreateProductFromFile</t>
   </si>
   <si>
@@ -95,9 +82,6 @@
   </si>
   <si>
     <t>model</t>
-  </si>
-  <si>
-    <t>C:\Dev\QuantSA\Scripts\EuropeanOption.cs</t>
   </si>
   <si>
     <t>C:\Dev\QuantSA\Scripts\IncentiveOptionExample.cs</t>
@@ -113,7 +97,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,14 +114,6 @@
     </font>
     <font>
       <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -189,7 +165,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -199,8 +175,6 @@
     <xf numFmtId="15" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="15" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
@@ -535,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,7 +525,7 @@
   <sheetData>
     <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -559,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
@@ -567,13 +541,13 @@
         <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="str">
         <f>_xll.QSA.CreateProductFromFile(C3,C4)</f>
-        <v>simpleCallFromFile.11:42:19-14</v>
+        <v>simpleCallFromFile.06:50:11-2</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="21" x14ac:dyDescent="0.35">
@@ -592,40 +566,40 @@
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="11">
+        <v>20</v>
+      </c>
+      <c r="C13" s="9">
         <f>Model!M6</f>
         <v>42643</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C14" s="1" t="str">
         <f>Model!B11</f>
-        <v>equitySimulator01.11:42:19-15</v>
+        <v>equitySimulator01.06:50:11-4</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="10">
         <v>50000</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="str">
         <f>_xll.QSA.Value(C12,B8,C13,C14,C15)</f>
-        <v>simpleCallFromFileValue.11:42:20-18</v>
+        <v>simpleCallFromFileValue.06:50:11-5</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="8">
         <f>_xll.QSA.GetResults(B17,"value")</f>
-        <v>1.5451465707928331</v>
+        <v>1.5538815913526058</v>
       </c>
     </row>
   </sheetData>
@@ -635,114 +609,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="B3" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="str">
-        <f>_xll.QSA.CreateProductFromFile(C4,C5)</f>
-        <v>productFromFile.11:42:20-17</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="B12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="2" t="str">
-        <f>C4&amp;"Value"</f>
-        <v>productFromFileValue</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="10">
-        <v>42975</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="2">
-        <v>100000</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="9">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G15" s="8">
-        <f>_xll.QSA.FormulaBlackScholes(G14,Model!M6,G13,Model!C8,Model!D8,Model!N6,Model!E8)</f>
-        <v>1.6117342518139377</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="str">
-        <f>_xll.QSA.Value(C13,B9,Model!M6,Model!B11,C14)</f>
-        <v>productFromFileValue.11:42:21-20</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="8">
-        <f>_xll.QSA.GetResults(B16,"value")</f>
-        <v>1.6201430965076</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
@@ -758,7 +627,7 @@
   <sheetData>
     <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -766,7 +635,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
@@ -774,13 +643,13 @@
         <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="str">
         <f>_xll.QSA.CreateProductFromFile(C3,C4)</f>
-        <v>incentiveOptionFromFile.11:42:20-16</v>
+        <v>incentiveOptionFromFile.06:50:11-3</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="21" x14ac:dyDescent="0.35">
@@ -799,40 +668,40 @@
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="11">
+        <v>20</v>
+      </c>
+      <c r="C13" s="9">
         <f>Model!M6</f>
         <v>42643</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C14" s="1" t="str">
         <f>Model!B11</f>
-        <v>equitySimulator01.11:42:19-15</v>
+        <v>equitySimulator01.06:50:11-4</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="10">
         <v>50000</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="str">
         <f>_xll.QSA.Value(C12,B8,C13,C14,C15)</f>
-        <v>incentiveOptionFromFileValue.11:42:20-19</v>
+        <v>incentiveOptionFromFileValue.06:50:11-6</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="8">
         <f>_xll.QSA.GetResults(B17,"value")</f>
-        <v>34.538951123841137</v>
+        <v>33.988116971237872</v>
       </c>
     </row>
   </sheetData>
@@ -840,7 +709,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N11"/>
   <sheetViews>
@@ -885,7 +754,7 @@
       </c>
       <c r="C4" s="1" t="str">
         <f>M9</f>
-        <v>ZARDiscount.11:42:19-13</v>
+        <v>ZARDiscount.06:50:10-1</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>10</v>
@@ -993,13 +862,13 @@
       </c>
       <c r="M9" s="5" t="str">
         <f>_xll.QSA.CreateDatesAndRatesCurve(N3,M6:M7,N6:N7,N4)</f>
-        <v>ZARDiscount.11:42:19-13</v>
+        <v>ZARDiscount.06:50:10-1</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="str">
         <f>_xll.QSA.CreateEquityModel(C3,C4,B7:B9,C7:C9,D7:D9,E7:E9,G7:I9)</f>
-        <v>equitySimulator01.11:42:19-15</v>
+        <v>equitySimulator01.06:50:11-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Checks for release and updated library to be consistent with them.
</commit_message>
<xml_diff>
--- a/ExcelExamples/CreateProductFromFile.xlsx
+++ b/ExcelExamples/CreateProductFromFile.xlsx
@@ -63,9 +63,6 @@
     <t>QSA.CreateEquityModel</t>
   </si>
   <si>
-    <t>shareCode</t>
-  </si>
-  <si>
     <t>QSA.Value</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>simpleCallFromFile</t>
+  </si>
+  <si>
+    <t>filename</t>
   </si>
 </sst>
 </file>
@@ -510,7 +510,7 @@
   <dimension ref="B2:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,7 +525,7 @@
   <sheetData>
     <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -533,15 +533,15 @@
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
@@ -552,7 +552,7 @@
     </row>
     <row r="11" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B11" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
@@ -566,7 +566,7 @@
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="9">
         <f>Model!M6</f>
@@ -575,7 +575,7 @@
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="1" t="str">
         <f>Model!B11</f>
@@ -584,7 +584,7 @@
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="10">
         <v>50000</v>
@@ -612,7 +612,7 @@
   <dimension ref="B2:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,7 +627,7 @@
   <sheetData>
     <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -635,15 +635,15 @@
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
@@ -654,7 +654,7 @@
     </row>
     <row r="11" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B11" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
@@ -668,7 +668,7 @@
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="9">
         <f>Model!M6</f>
@@ -677,7 +677,7 @@
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="1" t="str">
         <f>Model!B11</f>
@@ -686,7 +686,7 @@
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="10">
         <v>50000</v>

</xml_diff>

<commit_message>
documentation on installing, addin tweaks before test release.
</commit_message>
<xml_diff>
--- a/ExcelExamples/CreateProductFromFile.xlsx
+++ b/ExcelExamples/CreateProductFromFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="10290" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="10290"/>
   </bookViews>
   <sheets>
     <sheet name="Script Call Simple" sheetId="5" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>name</t>
   </si>
@@ -79,12 +79,6 @@
   </si>
   <si>
     <t>model</t>
-  </si>
-  <si>
-    <t>C:\Dev\QuantSA\Scripts\IncentiveOptionExample.cs</t>
-  </si>
-  <si>
-    <t>C:\Dev\QuantSA\Scripts\EuropeanCallSimple.cs</t>
   </si>
   <si>
     <t>simpleCallFromFile</t>
@@ -509,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,21 +527,22 @@
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="2" t="s">
         <v>22</v>
+      </c>
+      <c r="C4" s="2" t="str">
+        <f>_xll.QSA.GetInstallPath()&amp;"\Scripts\EuropeanCallSimple.cs"</f>
+        <v>C:\Dev\QuantSA\QuantSA\ExcelAddin\bin\Debug\Scripts\EuropeanCallSimple.cs</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="str">
         <f>_xll.QSA.CreateProductFromFile(C3,C4)</f>
-        <v>simpleCallFromFile.06:50:11-2</v>
+        <v>simpleCallFromFile.08:33:51-14</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="21" x14ac:dyDescent="0.35">
@@ -579,7 +574,7 @@
       </c>
       <c r="C14" s="1" t="str">
         <f>Model!B11</f>
-        <v>equitySimulator01.06:50:11-4</v>
+        <v>equitySimulator01.08:33:51-15</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
@@ -593,13 +588,13 @@
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="str">
         <f>_xll.QSA.Value(C12,B8,C13,C14,C15)</f>
-        <v>simpleCallFromFileValue.06:50:11-5</v>
+        <v>simpleCallFromFileValue.08:33:52-17</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="8">
         <f>_xll.QSA.GetResults(B17,"value")</f>
-        <v>1.5538815913526058</v>
+        <v>1.606579093676912</v>
       </c>
     </row>
   </sheetData>
@@ -611,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,16 +635,17 @@
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="str">
+        <f>_xll.QSA.GetInstallPath()&amp;"\Scripts\IncentiveOptionExample.cs"</f>
+        <v>C:\Dev\QuantSA\QuantSA\ExcelAddin\bin\Debug\Scripts\IncentiveOptionExample.cs</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="str">
         <f>_xll.QSA.CreateProductFromFile(C3,C4)</f>
-        <v>incentiveOptionFromFile.06:50:11-3</v>
+        <v>incentiveOptionFromFile.08:33:51-16</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="21" x14ac:dyDescent="0.35">
@@ -681,7 +677,7 @@
       </c>
       <c r="C14" s="1" t="str">
         <f>Model!B11</f>
-        <v>equitySimulator01.06:50:11-4</v>
+        <v>equitySimulator01.08:33:51-15</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
@@ -695,13 +691,13 @@
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="str">
         <f>_xll.QSA.Value(C12,B8,C13,C14,C15)</f>
-        <v>incentiveOptionFromFileValue.06:50:11-6</v>
+        <v>incentiveOptionFromFileValue.08:33:52-18</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="8">
         <f>_xll.QSA.GetResults(B17,"value")</f>
-        <v>33.988116971237872</v>
+        <v>33.442599376362196</v>
       </c>
     </row>
   </sheetData>
@@ -754,7 +750,7 @@
       </c>
       <c r="C4" s="1" t="str">
         <f>M9</f>
-        <v>ZARDiscount.06:50:10-1</v>
+        <v>ZARDiscount.08:33:51-13</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>10</v>
@@ -862,13 +858,13 @@
       </c>
       <c r="M9" s="5" t="str">
         <f>_xll.QSA.CreateDatesAndRatesCurve(N3,M6:M7,N6:N7,N4)</f>
-        <v>ZARDiscount.06:50:10-1</v>
+        <v>ZARDiscount.08:33:51-13</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="str">
         <f>_xll.QSA.CreateEquityModel(C3,C4,B7:B9,C7:C9,D7:D9,E7:E9,G7:I9)</f>
-        <v>equitySimulator01.06:50:11-4</v>
+        <v>equitySimulator01.08:33:51-15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change share separator to '.'
</commit_message>
<xml_diff>
--- a/ExcelExamples/CreateProductFromFile.xlsx
+++ b/ExcelExamples/CreateProductFromFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="10290"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="10290" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Script Call Simple" sheetId="5" r:id="rId1"/>
@@ -39,15 +39,6 @@
     <t>correlations</t>
   </si>
   <si>
-    <t>ZAR:ALSI</t>
-  </si>
-  <si>
-    <t>ZAR:AAA</t>
-  </si>
-  <si>
-    <t>ZAR:BBB</t>
-  </si>
-  <si>
     <t>currency</t>
   </si>
   <si>
@@ -85,6 +76,15 @@
   </si>
   <si>
     <t>filename</t>
+  </si>
+  <si>
+    <t>ZAR.ALSI</t>
+  </si>
+  <si>
+    <t>ZAR.AAA</t>
+  </si>
+  <si>
+    <t>ZAR.BBB</t>
   </si>
 </sst>
 </file>
@@ -503,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,7 +519,7 @@
   <sheetData>
     <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -527,27 +527,27 @@
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2" t="str">
         <f>_xll.QSA.GetInstallPath()&amp;"\Scripts\EuropeanCallSimple.cs"</f>
-        <v>C:\Dev\QuantSA\QuantSA\ExcelAddin\bin\Debug\Scripts\EuropeanCallSimple.cs</v>
+        <v>C:\Dev\QuantSA\QuantSA\QuantSA.Excel.AddIn\bin\Debug\Scripts\EuropeanCallSimple.cs</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="str">
         <f>_xll.QSA.CreateProductFromFile(C3,C4)</f>
-        <v>simpleCallFromFile.08:33:51-14</v>
+        <v>simpleCallFromFile.19:48:33-5</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B11" s="7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
@@ -561,7 +561,7 @@
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C13" s="9">
         <f>Model!M6</f>
@@ -570,16 +570,16 @@
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C14" s="1" t="str">
         <f>Model!B11</f>
-        <v>equitySimulator01.08:33:51-15</v>
+        <v>equitySimulator01.19:48:33-6</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C15" s="10">
         <v>50000</v>
@@ -588,13 +588,13 @@
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="str">
         <f>_xll.QSA.Value(C12,B8,C13,C14,C15)</f>
-        <v>simpleCallFromFileValue.08:33:52-17</v>
+        <v>simpleCallFromFileValue.19:48:33-8</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="8">
         <f>_xll.QSA.GetResults(B17,"value")</f>
-        <v>1.606579093676912</v>
+        <v>1.6457880207682005</v>
       </c>
     </row>
   </sheetData>
@@ -622,7 +622,7 @@
   <sheetData>
     <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -630,27 +630,27 @@
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2" t="str">
         <f>_xll.QSA.GetInstallPath()&amp;"\Scripts\IncentiveOptionExample.cs"</f>
-        <v>C:\Dev\QuantSA\QuantSA\ExcelAddin\bin\Debug\Scripts\IncentiveOptionExample.cs</v>
+        <v>C:\Dev\QuantSA\QuantSA\QuantSA.Excel.AddIn\bin\Debug\Scripts\IncentiveOptionExample.cs</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="str">
         <f>_xll.QSA.CreateProductFromFile(C3,C4)</f>
-        <v>incentiveOptionFromFile.08:33:51-16</v>
+        <v>incentiveOptionFromFile.19:48:33-7</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B11" s="7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
@@ -664,7 +664,7 @@
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C13" s="9">
         <f>Model!M6</f>
@@ -673,16 +673,16 @@
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C14" s="1" t="str">
         <f>Model!B11</f>
-        <v>equitySimulator01.08:33:51-15</v>
+        <v>equitySimulator01.19:48:33-6</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C15" s="10">
         <v>50000</v>
@@ -691,13 +691,13 @@
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="str">
         <f>_xll.QSA.Value(C12,B8,C13,C14,C15)</f>
-        <v>incentiveOptionFromFileValue.08:33:52-18</v>
+        <v>incentiveOptionFromFileValue.19:48:34-9</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="8">
         <f>_xll.QSA.GetResults(B17,"value")</f>
-        <v>33.442599376362196</v>
+        <v>34.177287918907005</v>
       </c>
     </row>
   </sheetData>
@@ -709,8 +709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,7 +727,7 @@
   <sheetData>
     <row r="2" spans="2:14" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
@@ -735,13 +735,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
@@ -750,13 +750,13 @@
       </c>
       <c r="C4" s="1" t="str">
         <f>M9</f>
-        <v>ZARDiscount.08:33:51-13</v>
+        <v>ZARDiscount.19:48:33-4</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -784,7 +784,7 @@
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2">
         <v>200</v>
@@ -813,7 +813,7 @@
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C8" s="2">
         <v>50</v>
@@ -836,7 +836,7 @@
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C9" s="2">
         <v>100</v>
@@ -858,13 +858,13 @@
       </c>
       <c r="M9" s="5" t="str">
         <f>_xll.QSA.CreateDatesAndRatesCurve(N3,M6:M7,N6:N7,N4)</f>
-        <v>ZARDiscount.08:33:51-13</v>
+        <v>ZARDiscount.19:48:33-4</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="str">
         <f>_xll.QSA.CreateEquityModel(C3,C4,B7:B9,C7:C9,D7:D9,E7:E9,G7:I9)</f>
-        <v>equitySimulator01.08:33:51-15</v>
+        <v>equitySimulator01.19:48:33-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All excel tests passing
</commit_message>
<xml_diff>
--- a/ExcelExamples/CreateProductFromFile.xlsx
+++ b/ExcelExamples/CreateProductFromFile.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Script Incentive Option" sheetId="3" r:id="rId2"/>
     <sheet name="Model" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" calcMode="manual" calcOnSave="0"/>
+  <calcPr calcId="145621" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
 </workbook>
 </file>
 
@@ -542,7 +542,7 @@
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="str">
         <f>_xll.QSA.CreateProductFromFile(C3,C4)</f>
-        <v>simpleCallFromFile.19:48:33-5</v>
+        <v>simpleCallFromFile.20:08:36-88</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="21" x14ac:dyDescent="0.35">
@@ -574,7 +574,7 @@
       </c>
       <c r="C14" s="1" t="str">
         <f>Model!B11</f>
-        <v>equitySimulator01.19:48:33-6</v>
+        <v>ERROR: Object reference not set to an instance of an object.</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
@@ -588,13 +588,13 @@
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="str">
         <f>_xll.QSA.Value(C12,B8,C13,C14,C15)</f>
-        <v>simpleCallFromFileValue.19:48:33-8</v>
+        <v>ERROR: model: No converter for type: NumeraireSimulator and no object named ERROR: Object reference not set to an instance of an object. on the map.</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="8">
+      <c r="B18" s="8" t="str">
         <f>_xll.QSA.GetResults(B17,"value")</f>
-        <v>1.6457880207682005</v>
+        <v>ERROR: resultStore: No converter for type: IProvidesResultStore and no object named ERROR: model: No converter for type: NumeraireSimulator and no object named ERROR: Object reference not set to an instance of an object. on the map. on the map.</v>
       </c>
     </row>
   </sheetData>
@@ -607,7 +607,7 @@
   <dimension ref="B2:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,7 +645,7 @@
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="str">
         <f>_xll.QSA.CreateProductFromFile(C3,C4)</f>
-        <v>incentiveOptionFromFile.19:48:33-7</v>
+        <v>incentiveOptionFromFile.20:08:36-89</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="21" x14ac:dyDescent="0.35">
@@ -677,7 +677,7 @@
       </c>
       <c r="C14" s="1" t="str">
         <f>Model!B11</f>
-        <v>equitySimulator01.19:48:33-6</v>
+        <v>ERROR: Object reference not set to an instance of an object.</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
@@ -691,13 +691,13 @@
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="str">
         <f>_xll.QSA.Value(C12,B8,C13,C14,C15)</f>
-        <v>incentiveOptionFromFileValue.19:48:34-9</v>
+        <v>ERROR: model: No converter for type: NumeraireSimulator and no object named ERROR: Object reference not set to an instance of an object. on the map.</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="8">
+      <c r="B18" s="8" t="str">
         <f>_xll.QSA.GetResults(B17,"value")</f>
-        <v>34.177287918907005</v>
+        <v>ERROR: resultStore: No converter for type: IProvidesResultStore and no object named ERROR: model: No converter for type: NumeraireSimulator and no object named ERROR: Object reference not set to an instance of an object. on the map. on the map.</v>
       </c>
     </row>
   </sheetData>
@@ -710,7 +710,7 @@
   <dimension ref="B2:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,7 +750,7 @@
       </c>
       <c r="C4" s="1" t="str">
         <f>M9</f>
-        <v>ZARDiscount.19:48:33-4</v>
+        <v>ZARDiscount.20:08:36-87</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>7</v>
@@ -858,13 +858,13 @@
       </c>
       <c r="M9" s="5" t="str">
         <f>_xll.QSA.CreateDatesAndRatesCurve(N3,M6:M7,N6:N7,N4)</f>
-        <v>ZARDiscount.19:48:33-4</v>
+        <v>ZARDiscount.20:08:36-87</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="str">
-        <f>_xll.QSA.CreateEquityModel(C3,C4,B7:B9,C7:C9,D7:D9,E7:E9,G7:I9)</f>
-        <v>equitySimulator01.19:48:33-6</v>
+        <f ca="1">_xll.QSA.CreateEquityModel(C3,C4,B7:B9,C7:C9,D7:D9,E7:E9,G7:I9)</f>
+        <v>ERROR: Object reference not set to an instance of an object.</v>
       </c>
     </row>
   </sheetData>

</xml_diff>